<commit_message>
Fix bug and option arena
</commit_message>
<xml_diff>
--- a/src/assets/template/3-Mau_Tho_Doi_Khang.xlsx
+++ b/src/assets/template/3-Mau_Tho_Doi_Khang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Project\cocvuong-react\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Project\cocvuong.com\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F5FD6A-907E-46DB-8DE5-867EABC86E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315EE0F4-8CE9-47C1-8020-82B3E9EF6B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="14" r:id="rId1"/>
@@ -29,230 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="561">
-  <si>
-    <t>Nguyễn Thành Nhân</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="498">
   <si>
     <t>55kg nam</t>
   </si>
   <si>
-    <t>Trần Lê Minh</t>
-  </si>
-  <si>
-    <t>FPT University (A)</t>
-  </si>
-  <si>
-    <t>Lý Quang Lưu</t>
-  </si>
-  <si>
-    <t>CĐ FPT Poly (CĐ Anh Quốc) (A)</t>
-  </si>
-  <si>
-    <t>Hoàng Duy Anh</t>
-  </si>
-  <si>
-    <t>Phạm Mai Nhật Trường</t>
-  </si>
-  <si>
-    <t>Greenwich (Việt Nam) (A)</t>
-  </si>
-  <si>
-    <t>Nguyễn Phúc Long</t>
-  </si>
-  <si>
-    <t>Trần Minh Phụng</t>
-  </si>
-  <si>
-    <t>60kg nam</t>
-  </si>
-  <si>
-    <t>Võ Minh Hiền</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đinh Hoàng Danh </t>
-  </si>
-  <si>
-    <t>Lê Đức Trọng</t>
-  </si>
-  <si>
-    <t>Nguyễn Bảo Phú</t>
-  </si>
-  <si>
-    <t>50kg nữ</t>
-  </si>
-  <si>
-    <t>Phạm Thị Thanh Phương</t>
-  </si>
-  <si>
-    <t>Swinburne (Việt Nam) (A)</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Hồng Yên</t>
-  </si>
-  <si>
-    <t>Lê Đắc Lợi</t>
-  </si>
-  <si>
-    <t>Nguyễn Đức Huy</t>
-  </si>
-  <si>
-    <t>Phan Nguyễn Quang Khang</t>
-  </si>
-  <si>
-    <t>Nguyễn Xuân Khang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Linh Cảnh </t>
-  </si>
-  <si>
-    <t>Hồ Viết Thuận</t>
-  </si>
-  <si>
-    <t>Cao đẳng FPT Polytechnic (A)</t>
-  </si>
-  <si>
-    <t>Đặng Quốc Tuân</t>
-  </si>
-  <si>
-    <t>Trương Công Tuệ Tĩnh</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Bình</t>
-  </si>
-  <si>
-    <t>Nguyễn Thái Vĩnh</t>
-  </si>
-  <si>
-    <t>Nguyễn Bình Ca</t>
-  </si>
-  <si>
-    <t>65kg nam</t>
-  </si>
-  <si>
-    <t>Lưu Triều Lễ</t>
-  </si>
-  <si>
-    <t>Nguyễn Công Tài</t>
-  </si>
-  <si>
-    <t>Nguyễn Hoàng Long</t>
-  </si>
-  <si>
-    <t>Lê Trung Tiến</t>
-  </si>
-  <si>
-    <t>Đỗ Nguyễn Đăng Khoa</t>
-  </si>
-  <si>
-    <t>Cao Trí Tưởng</t>
-  </si>
-  <si>
-    <t>70kg nam</t>
-  </si>
-  <si>
-    <t>Ngô Nguyễn Thanh Phong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Hoàng Thuận </t>
-  </si>
-  <si>
-    <t>Dương Quý Thành</t>
-  </si>
-  <si>
-    <t>Mạc Đăng Hải</t>
-  </si>
-  <si>
-    <t>Hoàng Minh Tiến</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Quốc Đạt </t>
-  </si>
-  <si>
-    <t>Bùi Vĩnh Lộc</t>
-  </si>
-  <si>
-    <t>75kg nam</t>
-  </si>
-  <si>
-    <t>Cao Hoàng Duy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lê Hoàng Hải </t>
-  </si>
-  <si>
-    <t>Lê Trần Minh Đạt</t>
-  </si>
-  <si>
-    <t>Nguyễn Anh Minh</t>
-  </si>
-  <si>
-    <t>45kg nữ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đặng Thị Huyền </t>
-  </si>
-  <si>
-    <t>Nguyễn Huỳnh Mai Ngân</t>
-  </si>
-  <si>
-    <t>Nguyễn Thanh Vân</t>
-  </si>
-  <si>
-    <t>Hồ Phương Vy</t>
-  </si>
-  <si>
-    <t>Trần Phạm Hà My</t>
-  </si>
-  <si>
-    <t>60kg nữ</t>
-  </si>
-  <si>
-    <t>Võ Thị Hiền Duyên</t>
-  </si>
-  <si>
-    <t>Lê Ngọc Đông Nghi</t>
-  </si>
-  <si>
-    <t>65kg nữ</t>
-  </si>
-  <si>
-    <t>Nguyễn Ngọc Minh Thy</t>
-  </si>
-  <si>
-    <t>Võ Bùi Hải Nguyên</t>
-  </si>
-  <si>
-    <t>Trần Gia Quyên</t>
-  </si>
-  <si>
-    <t>Trần Nhật Anh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Tấn Đạt </t>
-  </si>
-  <si>
-    <t>Phạm Ngọc Phương Nhi</t>
-  </si>
-  <si>
-    <t>55kg nữ</t>
-  </si>
-  <si>
-    <t>Phạm Thanh Hiền</t>
-  </si>
-  <si>
-    <t>Trần Thị Minh Thư</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trần Thị Kim Oanh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">65kg nữ </t>
-  </si>
-  <si>
-    <t>Đặng Nguyễn Xuân Thy</t>
-  </si>
-  <si>
     <t>HẠNG CÂN</t>
   </si>
   <si>
@@ -1712,6 +1493,36 @@
   </si>
   <si>
     <t>QUỐC GIA</t>
+  </si>
+  <si>
+    <t>Vận Động Viên 1</t>
+  </si>
+  <si>
+    <t>Vận Động Viên 2</t>
+  </si>
+  <si>
+    <t>Vận Động Viên 3</t>
+  </si>
+  <si>
+    <t>Vận Động Viên 4</t>
+  </si>
+  <si>
+    <t>Vận Động Viên 5</t>
+  </si>
+  <si>
+    <t>Đơn vị 1</t>
+  </si>
+  <si>
+    <t>Đơn vị 2</t>
+  </si>
+  <si>
+    <t>Đơn vị 3</t>
+  </si>
+  <si>
+    <t>Đơn vị 4</t>
+  </si>
+  <si>
+    <t>Đơn vị 5</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +1915,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061F8C4D-20A2-47D9-8BDD-D68431096479}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2119,19 +1930,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>560</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2139,16 +1950,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>488</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>493</v>
       </c>
       <c r="E2" t="s">
-        <v>463</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2156,16 +1967,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>489</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>494</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2173,16 +1984,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>490</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>495</v>
       </c>
       <c r="E4" t="s">
-        <v>463</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2190,16 +2001,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>491</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>496</v>
       </c>
       <c r="E5" t="s">
-        <v>463</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2207,929 +2018,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>492</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>497</v>
       </c>
       <c r="E6" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>39</v>
-      </c>
-      <c r="C52" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>47</v>
-      </c>
-      <c r="C54" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>52</v>
-      </c>
-      <c r="C55" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" t="s">
-        <v>3</v>
-      </c>
-      <c r="E55" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>58</v>
-      </c>
-      <c r="C57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>68</v>
-      </c>
-      <c r="C59" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" t="s">
-        <v>463</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D1C45E4-D1EC-40A3-9DCD-FF23338A62A5}">
           <x14:formula1>
             <xm:f>quocgia!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E59</xm:sqref>
+          <xm:sqref>E2:E6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3141,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA5013A-5829-445E-BA15-779565CF825F}">
   <dimension ref="A1:C241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3154,10 +2064,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3165,10 +2075,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3176,10 +2086,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3187,10 +2097,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3198,10 +2108,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>470</v>
+        <v>397</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>471</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3209,10 +2119,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3220,10 +2130,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,10 +2141,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>472</v>
+        <v>399</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>473</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3242,10 +2152,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>474</v>
+        <v>401</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>475</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3253,10 +2163,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3264,10 +2174,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3275,10 +2185,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3286,10 +2196,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>476</v>
+        <v>403</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>477</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3297,10 +2207,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,10 +2218,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,10 +2229,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3330,10 +2240,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3341,10 +2251,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3352,10 +2262,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3363,10 +2273,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3374,10 +2284,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3385,10 +2295,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3396,10 +2306,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3407,10 +2317,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3418,10 +2328,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>478</v>
+        <v>405</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>479</v>
+        <v>406</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3429,10 +2339,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3440,10 +2350,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>120</v>
+        <v>47</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3451,10 +2361,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,10 +2372,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3473,10 +2383,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>127</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3484,10 +2394,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>480</v>
+        <v>407</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>481</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3495,10 +2405,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>482</v>
+        <v>409</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>483</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3506,10 +2416,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>128</v>
+        <v>55</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3517,10 +2427,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>131</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3528,10 +2438,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>132</v>
+        <v>59</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>133</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3539,10 +2449,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>135</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,10 +2460,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>137</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3561,10 +2471,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3572,10 +2482,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3583,10 +2493,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3594,10 +2504,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>484</v>
+        <v>411</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>485</v>
+        <v>412</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3605,10 +2515,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>145</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3616,10 +2526,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>146</v>
+        <v>73</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>147</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3627,10 +2537,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3638,10 +2548,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>150</v>
+        <v>77</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3649,10 +2559,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>486</v>
+        <v>413</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>487</v>
+        <v>414</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3660,10 +2570,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>488</v>
+        <v>415</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>489</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3671,10 +2581,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3682,10 +2592,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>155</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3693,10 +2603,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3704,10 +2614,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>490</v>
+        <v>417</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>491</v>
+        <v>418</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3715,10 +2625,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3726,10 +2636,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>160</v>
+        <v>87</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>161</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3737,10 +2647,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>162</v>
+        <v>89</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3748,10 +2658,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>164</v>
+        <v>91</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>165</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3759,10 +2669,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>492</v>
+        <v>419</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>493</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3770,10 +2680,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>167</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3781,10 +2691,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>169</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3792,10 +2702,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3803,10 +2713,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>172</v>
+        <v>99</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>173</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3814,10 +2724,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>174</v>
+        <v>101</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>175</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3825,10 +2735,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>176</v>
+        <v>103</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>177</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3836,10 +2746,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>178</v>
+        <v>105</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>179</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3847,10 +2757,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>180</v>
+        <v>107</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3858,10 +2768,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3869,10 +2779,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>184</v>
+        <v>111</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>185</v>
+        <v>112</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3880,10 +2790,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>187</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3891,10 +2801,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>188</v>
+        <v>115</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>189</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3902,10 +2812,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>190</v>
+        <v>117</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>191</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3913,10 +2823,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>192</v>
+        <v>119</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>193</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3924,10 +2834,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>194</v>
+        <v>121</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>195</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3935,10 +2845,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>494</v>
+        <v>421</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>495</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3946,10 +2856,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>496</v>
+        <v>423</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>497</v>
+        <v>424</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3957,10 +2867,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>196</v>
+        <v>123</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>197</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3968,10 +2878,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>199</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3979,10 +2889,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>200</v>
+        <v>127</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>201</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3990,10 +2900,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>498</v>
+        <v>425</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>499</v>
+        <v>426</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -4001,10 +2911,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>202</v>
+        <v>129</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>203</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -4012,10 +2922,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>204</v>
+        <v>131</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>205</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -4023,10 +2933,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>207</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -4034,10 +2944,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>208</v>
+        <v>135</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>209</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -4045,10 +2955,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>210</v>
+        <v>137</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>211</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -4056,10 +2966,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>500</v>
+        <v>427</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>501</v>
+        <v>428</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -4067,10 +2977,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>212</v>
+        <v>139</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>213</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -4078,10 +2988,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>502</v>
+        <v>429</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>503</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -4089,10 +2999,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>214</v>
+        <v>141</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>215</v>
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -4100,10 +3010,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>504</v>
+        <v>431</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>505</v>
+        <v>432</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -4111,10 +3021,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>216</v>
+        <v>143</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>217</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -4122,10 +3032,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>506</v>
+        <v>433</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>507</v>
+        <v>434</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -4133,10 +3043,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>219</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -4144,10 +3054,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>220</v>
+        <v>147</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>221</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -4155,10 +3065,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>222</v>
+        <v>149</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>223</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -4166,10 +3076,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>224</v>
+        <v>151</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>225</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -4177,10 +3087,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>226</v>
+        <v>153</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>227</v>
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -4188,10 +3098,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>228</v>
+        <v>155</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>229</v>
+        <v>156</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -4199,10 +3109,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>508</v>
+        <v>435</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>509</v>
+        <v>436</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -4210,10 +3120,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>230</v>
+        <v>157</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>231</v>
+        <v>158</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -4221,10 +3131,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>233</v>
+        <v>160</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -4232,10 +3142,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>234</v>
+        <v>161</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>235</v>
+        <v>162</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -4243,10 +3153,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>236</v>
+        <v>163</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>237</v>
+        <v>164</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -4254,10 +3164,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>238</v>
+        <v>165</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4265,10 +3175,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>240</v>
+        <v>167</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>241</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -4276,10 +3186,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>242</v>
+        <v>169</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>243</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -4287,10 +3197,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>510</v>
+        <v>437</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>511</v>
+        <v>438</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -4298,10 +3208,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>244</v>
+        <v>171</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -4309,10 +3219,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>246</v>
+        <v>173</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>247</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -4320,10 +3230,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>248</v>
+        <v>175</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>249</v>
+        <v>176</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -4331,10 +3241,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>250</v>
+        <v>177</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>251</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4342,10 +3252,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>512</v>
+        <v>439</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>513</v>
+        <v>440</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4353,10 +3263,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>252</v>
+        <v>179</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>253</v>
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -4364,10 +3274,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>254</v>
+        <v>181</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>255</v>
+        <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -4375,10 +3285,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>256</v>
+        <v>183</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>257</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -4386,10 +3296,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>258</v>
+        <v>185</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>259</v>
+        <v>186</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -4397,10 +3307,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>514</v>
+        <v>441</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>515</v>
+        <v>442</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -4408,10 +3318,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>260</v>
+        <v>187</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>261</v>
+        <v>188</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -4419,10 +3329,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>262</v>
+        <v>189</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>263</v>
+        <v>190</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -4430,10 +3340,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>264</v>
+        <v>191</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>265</v>
+        <v>192</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -4441,10 +3351,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>266</v>
+        <v>193</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>267</v>
+        <v>194</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -4452,10 +3362,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>268</v>
+        <v>195</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>269</v>
+        <v>196</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -4463,10 +3373,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>270</v>
+        <v>197</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>271</v>
+        <v>198</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -4474,10 +3384,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>272</v>
+        <v>199</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>273</v>
+        <v>200</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -4485,10 +3395,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>274</v>
+        <v>201</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>275</v>
+        <v>202</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4496,10 +3406,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>276</v>
+        <v>203</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>277</v>
+        <v>204</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4507,10 +3417,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>278</v>
+        <v>205</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>279</v>
+        <v>206</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4518,10 +3428,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>280</v>
+        <v>207</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>281</v>
+        <v>208</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -4529,10 +3439,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>516</v>
+        <v>443</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>517</v>
+        <v>444</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -4540,10 +3450,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>282</v>
+        <v>209</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>283</v>
+        <v>210</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4551,10 +3461,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>284</v>
+        <v>211</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>285</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4562,10 +3472,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>286</v>
+        <v>213</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>287</v>
+        <v>214</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4573,10 +3483,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>288</v>
+        <v>215</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>289</v>
+        <v>216</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -4584,10 +3494,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>290</v>
+        <v>217</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>291</v>
+        <v>218</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4595,10 +3505,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>292</v>
+        <v>219</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -4606,10 +3516,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>294</v>
+        <v>221</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>295</v>
+        <v>222</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -4617,10 +3527,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>296</v>
+        <v>223</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>297</v>
+        <v>224</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -4628,10 +3538,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>298</v>
+        <v>225</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>299</v>
+        <v>226</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -4639,10 +3549,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>518</v>
+        <v>445</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>519</v>
+        <v>446</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -4650,10 +3560,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>301</v>
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -4661,10 +3571,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>302</v>
+        <v>229</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>303</v>
+        <v>230</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -4672,10 +3582,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>304</v>
+        <v>231</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>305</v>
+        <v>232</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -4683,10 +3593,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>306</v>
+        <v>233</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>307</v>
+        <v>234</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -4694,10 +3604,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>308</v>
+        <v>235</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>309</v>
+        <v>236</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4705,10 +3615,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>310</v>
+        <v>237</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>311</v>
+        <v>238</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4716,10 +3626,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>520</v>
+        <v>447</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>521</v>
+        <v>448</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -4727,10 +3637,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>312</v>
+        <v>239</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>313</v>
+        <v>240</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4738,10 +3648,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>314</v>
+        <v>241</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>315</v>
+        <v>242</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -4749,10 +3659,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>316</v>
+        <v>243</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>317</v>
+        <v>244</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -4760,10 +3670,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>318</v>
+        <v>245</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>319</v>
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -4771,10 +3681,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>320</v>
+        <v>247</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>321</v>
+        <v>248</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4782,10 +3692,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>322</v>
+        <v>249</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>323</v>
+        <v>250</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -4793,10 +3703,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>324</v>
+        <v>251</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>325</v>
+        <v>252</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4804,10 +3714,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>522</v>
+        <v>449</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>523</v>
+        <v>450</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -4815,10 +3725,10 @@
         <v>151</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>524</v>
+        <v>451</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>525</v>
+        <v>452</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4826,10 +3736,10 @@
         <v>152</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>326</v>
+        <v>253</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>327</v>
+        <v>254</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -4837,10 +3747,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>328</v>
+        <v>255</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>329</v>
+        <v>256</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4848,10 +3758,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>330</v>
+        <v>257</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>331</v>
+        <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4859,10 +3769,10 @@
         <v>155</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>332</v>
+        <v>259</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>333</v>
+        <v>260</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4870,10 +3780,10 @@
         <v>156</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>526</v>
+        <v>453</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>527</v>
+        <v>454</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4881,10 +3791,10 @@
         <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>334</v>
+        <v>261</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>335</v>
+        <v>262</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -4892,10 +3802,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>336</v>
+        <v>263</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>337</v>
+        <v>264</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4903,10 +3813,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>528</v>
+        <v>455</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>529</v>
+        <v>456</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -4914,10 +3824,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>338</v>
+        <v>265</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>339</v>
+        <v>266</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4925,10 +3835,10 @@
         <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>340</v>
+        <v>267</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>341</v>
+        <v>268</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4936,10 +3846,10 @@
         <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>342</v>
+        <v>269</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>343</v>
+        <v>270</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4947,10 +3857,10 @@
         <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>344</v>
+        <v>271</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>345</v>
+        <v>272</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -4958,10 +3868,10 @@
         <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>346</v>
+        <v>273</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>347</v>
+        <v>274</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -4969,10 +3879,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>348</v>
+        <v>275</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>349</v>
+        <v>276</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -4980,10 +3890,10 @@
         <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>350</v>
+        <v>277</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>351</v>
+        <v>278</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -4991,10 +3901,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>352</v>
+        <v>279</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>353</v>
+        <v>280</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -5002,10 +3912,10 @@
         <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>354</v>
+        <v>281</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>355</v>
+        <v>282</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -5013,10 +3923,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>530</v>
+        <v>457</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>531</v>
+        <v>458</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -5024,10 +3934,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>356</v>
+        <v>283</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>357</v>
+        <v>284</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -5035,10 +3945,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>358</v>
+        <v>285</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>359</v>
+        <v>286</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -5046,10 +3956,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>532</v>
+        <v>459</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>533</v>
+        <v>460</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -5057,10 +3967,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>360</v>
+        <v>287</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>361</v>
+        <v>288</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -5068,10 +3978,10 @@
         <v>174</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>534</v>
+        <v>461</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>535</v>
+        <v>462</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -5079,10 +3989,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>362</v>
+        <v>289</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>363</v>
+        <v>290</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -5090,10 +4000,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>364</v>
+        <v>291</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>365</v>
+        <v>292</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -5101,10 +4011,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>366</v>
+        <v>293</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>367</v>
+        <v>294</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -5112,10 +4022,10 @@
         <v>178</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>536</v>
+        <v>463</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>537</v>
+        <v>464</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -5123,10 +4033,10 @@
         <v>179</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>538</v>
+        <v>465</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>539</v>
+        <v>466</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -5134,10 +4044,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>368</v>
+        <v>295</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>369</v>
+        <v>296</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -5145,10 +4055,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>370</v>
+        <v>297</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>371</v>
+        <v>298</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -5156,10 +4066,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>540</v>
+        <v>467</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>541</v>
+        <v>468</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -5167,10 +4077,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>542</v>
+        <v>469</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>543</v>
+        <v>470</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -5178,10 +4088,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>372</v>
+        <v>299</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>373</v>
+        <v>300</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -5189,10 +4099,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>374</v>
+        <v>301</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>375</v>
+        <v>302</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -5200,10 +4110,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>376</v>
+        <v>303</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>377</v>
+        <v>304</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -5211,10 +4121,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>378</v>
+        <v>305</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>379</v>
+        <v>306</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -5222,10 +4132,10 @@
         <v>188</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>380</v>
+        <v>307</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>381</v>
+        <v>308</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -5233,10 +4143,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>382</v>
+        <v>309</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>383</v>
+        <v>310</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -5244,10 +4154,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>384</v>
+        <v>311</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>385</v>
+        <v>312</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -5255,10 +4165,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>386</v>
+        <v>313</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>387</v>
+        <v>314</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -5266,10 +4176,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>388</v>
+        <v>315</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>389</v>
+        <v>316</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -5277,10 +4187,10 @@
         <v>193</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>544</v>
+        <v>471</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>545</v>
+        <v>472</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -5288,10 +4198,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>390</v>
+        <v>317</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>391</v>
+        <v>318</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -5299,10 +4209,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>392</v>
+        <v>319</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>393</v>
+        <v>320</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -5310,10 +4220,10 @@
         <v>196</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>394</v>
+        <v>321</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>395</v>
+        <v>322</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -5321,10 +4231,10 @@
         <v>197</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>396</v>
+        <v>323</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>397</v>
+        <v>324</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -5332,10 +4242,10 @@
         <v>198</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>398</v>
+        <v>325</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>399</v>
+        <v>326</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -5343,10 +4253,10 @@
         <v>199</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>400</v>
+        <v>327</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>401</v>
+        <v>328</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -5354,10 +4264,10 @@
         <v>200</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>402</v>
+        <v>329</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>403</v>
+        <v>330</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -5365,10 +4275,10 @@
         <v>201</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>404</v>
+        <v>331</v>
       </c>
       <c r="C202" s="3" t="s">
-        <v>405</v>
+        <v>332</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -5376,10 +4286,10 @@
         <v>202</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>406</v>
+        <v>333</v>
       </c>
       <c r="C203" s="3" t="s">
-        <v>407</v>
+        <v>334</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -5387,10 +4297,10 @@
         <v>203</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>408</v>
+        <v>335</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>409</v>
+        <v>336</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -5398,10 +4308,10 @@
         <v>204</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>410</v>
+        <v>337</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>411</v>
+        <v>338</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -5409,10 +4319,10 @@
         <v>205</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>412</v>
+        <v>339</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>413</v>
+        <v>340</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -5420,10 +4330,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>414</v>
+        <v>341</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>415</v>
+        <v>342</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -5431,10 +4341,10 @@
         <v>207</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>546</v>
+        <v>473</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>547</v>
+        <v>474</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -5442,10 +4352,10 @@
         <v>208</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>416</v>
+        <v>343</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>417</v>
+        <v>344</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -5453,10 +4363,10 @@
         <v>209</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>418</v>
+        <v>345</v>
       </c>
       <c r="C210" s="3" t="s">
-        <v>419</v>
+        <v>346</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -5464,10 +4374,10 @@
         <v>210</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>420</v>
+        <v>347</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>421</v>
+        <v>348</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -5475,10 +4385,10 @@
         <v>211</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>548</v>
+        <v>475</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>549</v>
+        <v>476</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -5486,10 +4396,10 @@
         <v>212</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>422</v>
+        <v>349</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>423</v>
+        <v>350</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -5497,10 +4407,10 @@
         <v>213</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>424</v>
+        <v>351</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>425</v>
+        <v>352</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -5508,10 +4418,10 @@
         <v>214</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>426</v>
+        <v>353</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>427</v>
+        <v>354</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -5519,10 +4429,10 @@
         <v>215</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>428</v>
+        <v>355</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>429</v>
+        <v>356</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -5530,10 +4440,10 @@
         <v>216</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>430</v>
+        <v>357</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>431</v>
+        <v>358</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -5541,10 +4451,10 @@
         <v>217</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>550</v>
+        <v>477</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>551</v>
+        <v>478</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -5552,10 +4462,10 @@
         <v>218</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>432</v>
+        <v>359</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>433</v>
+        <v>360</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -5563,10 +4473,10 @@
         <v>219</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>434</v>
+        <v>361</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>435</v>
+        <v>362</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -5574,10 +4484,10 @@
         <v>220</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>436</v>
+        <v>363</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>437</v>
+        <v>364</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -5585,10 +4495,10 @@
         <v>221</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>438</v>
+        <v>365</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>439</v>
+        <v>366</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -5596,10 +4506,10 @@
         <v>222</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>440</v>
+        <v>367</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>441</v>
+        <v>368</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -5607,10 +4517,10 @@
         <v>223</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>552</v>
+        <v>479</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>553</v>
+        <v>480</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -5618,10 +4528,10 @@
         <v>224</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>442</v>
+        <v>369</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>443</v>
+        <v>370</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -5629,10 +4539,10 @@
         <v>225</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>554</v>
+        <v>481</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>555</v>
+        <v>482</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -5640,10 +4550,10 @@
         <v>226</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>444</v>
+        <v>371</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>445</v>
+        <v>372</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -5651,10 +4561,10 @@
         <v>227</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>446</v>
+        <v>373</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>447</v>
+        <v>374</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -5662,10 +4572,10 @@
         <v>228</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>448</v>
+        <v>375</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>449</v>
+        <v>376</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -5673,10 +4583,10 @@
         <v>229</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>450</v>
+        <v>377</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>451</v>
+        <v>378</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -5684,10 +4594,10 @@
         <v>230</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>452</v>
+        <v>379</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>453</v>
+        <v>380</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -5695,10 +4605,10 @@
         <v>231</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>454</v>
+        <v>381</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>455</v>
+        <v>382</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -5706,10 +4616,10 @@
         <v>232</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>456</v>
+        <v>383</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>457</v>
+        <v>384</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -5717,10 +4627,10 @@
         <v>233</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>458</v>
+        <v>385</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>459</v>
+        <v>386</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -5728,10 +4638,10 @@
         <v>234</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>460</v>
+        <v>387</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>461</v>
+        <v>388</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -5739,10 +4649,10 @@
         <v>235</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>462</v>
+        <v>389</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>463</v>
+        <v>390</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -5750,10 +4660,10 @@
         <v>236</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>556</v>
+        <v>483</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>557</v>
+        <v>484</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -5761,10 +4671,10 @@
         <v>237</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>558</v>
+        <v>485</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>559</v>
+        <v>486</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -5772,10 +4682,10 @@
         <v>238</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>464</v>
+        <v>391</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>465</v>
+        <v>392</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -5783,10 +4693,10 @@
         <v>239</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>466</v>
+        <v>393</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>467</v>
+        <v>394</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -5794,10 +4704,10 @@
         <v>240</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>468</v>
+        <v>395</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>469</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>